<commit_message>
test case binding and test listeners
</commit_message>
<xml_diff>
--- a/Data Files/DD_Login.xlsx
+++ b/Data Files/DD_Login.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lope112166\Katalon Studio\PT\Data Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lope112166\Katalon Studio\katalonbasic\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>XLS_Usuario</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>siigo@tech.com</t>
+  </si>
+  <si>
+    <t>tech@siigo.copm</t>
+  </si>
+  <si>
+    <t>tech@siigo.com</t>
   </si>
 </sst>
 </file>
@@ -368,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -403,10 +409,19 @@
         <v>1111</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>2222</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" location="/license"/>
     <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -414,10 +429,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,9 +457,18 @@
         <v>1112</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>1111</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>